<commit_message>
de nouvelles modifications pour les IVG : modification du type des dates (c au lieu de dmy)
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RSA IVG 17.xlsx
+++ b/formats/excel/Formats RSA IVG 17.xlsx
@@ -52,43 +52,43 @@
     <t xml:space="preserve">NOFINESSGEO</t>
   </si>
   <si>
-    <t xml:space="preserve">N° FINESS du fichier d'entrée 9 10 18</t>
+    <t xml:space="preserve">N° FINESS du fichier d'entrée</t>
   </si>
   <si>
     <t xml:space="preserve">TYPEPREST</t>
   </si>
   <si>
-    <t xml:space="preserve">Type de prestation 2 19 20</t>
+    <t xml:space="preserve">Type de prestation</t>
   </si>
   <si>
     <t xml:space="preserve">ANNEE</t>
   </si>
   <si>
-    <t xml:space="preserve">Année période 4 21 24</t>
+    <t xml:space="preserve">Année période</t>
   </si>
   <si>
     <t xml:space="preserve">MOIS</t>
   </si>
   <si>
-    <t xml:space="preserve">N° période (mois) 2 25 26</t>
+    <t xml:space="preserve">N° période (mois)</t>
   </si>
   <si>
     <t xml:space="preserve">CLE_RSA</t>
   </si>
   <si>
-    <t xml:space="preserve">N° d'index du RSA 10 27 36</t>
+    <t xml:space="preserve">N° d'index du RSA</t>
   </si>
   <si>
     <t xml:space="preserve">MOISSEJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Mois du séjour 2 37 38</t>
+    <t xml:space="preserve">Mois du séjour</t>
   </si>
   <si>
     <t xml:space="preserve">ANSEJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Année du séjour 4 39 42</t>
+    <t xml:space="preserve">Année du séjour</t>
   </si>
   <si>
     <t xml:space="preserve">NBIVGANT</t>
@@ -97,25 +97,25 @@
     <t xml:space="preserve">i</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre d'IVG antérieures 2 43 44</t>
+    <t xml:space="preserve">Nombre d'IVG antérieures</t>
   </si>
   <si>
     <t xml:space="preserve">ANIVGPREC</t>
   </si>
   <si>
-    <t xml:space="preserve">Année de la dernière IVG 4 45 48</t>
+    <t xml:space="preserve">Année de la dernière IVG</t>
   </si>
   <si>
     <t xml:space="preserve">NBNAIVIVANT</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre de naissances vivantes antérieures 2 49 50</t>
+    <t xml:space="preserve">Nombre de naissances vivantes antérieures</t>
   </si>
   <si>
     <t xml:space="preserve">Fil</t>
   </si>
   <si>
-    <t xml:space="preserve">Filler 30 51 80</t>
+    <t xml:space="preserve">Filler</t>
   </si>
 </sst>
 </file>
@@ -231,10 +231,10 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.88"/>

</xml_diff>